<commit_message>
File update and script update
</commit_message>
<xml_diff>
--- a/data/AllRetentostatData.xlsx
+++ b/data/AllRetentostatData.xlsx
@@ -1,26 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ben-c\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F702F56C-6444-46F8-9D6A-0B7DD8C36EB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E76F1D6-9D37-40AA-AD92-DAB677530599}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4920" yWindow="10755" windowWidth="11415" windowHeight="7380" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="C023" sheetId="5" r:id="rId1"/>
     <sheet name="C024" sheetId="7" r:id="rId2"/>
     <sheet name="C030" sheetId="9" r:id="rId3"/>
-    <sheet name="C097" sheetId="10" r:id="rId4"/>
-    <sheet name="C098" sheetId="11" r:id="rId5"/>
-    <sheet name="C025" sheetId="12" r:id="rId6"/>
-    <sheet name="C026" sheetId="13" r:id="rId7"/>
-    <sheet name="C029" sheetId="14" r:id="rId8"/>
+    <sheet name="C025" sheetId="12" r:id="rId4"/>
+    <sheet name="C026" sheetId="13" r:id="rId5"/>
+    <sheet name="C029" sheetId="14" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="17">
   <si>
     <t>V_A</t>
   </si>
@@ -99,21 +97,14 @@
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Courier New"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -261,7 +252,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -287,111 +278,97 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="14" fillId="8" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="9" borderId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0"/>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="0"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="10" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="3" fillId="0" borderId="2" xfId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="2" xfId="33" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -460,9 +437,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -500,9 +477,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -535,26 +512,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -587,26 +547,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1268,7 +1211,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF0531D9-B614-4E8C-B94A-D5501448ABF9}">
   <dimension ref="B2:L33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -2175,920 +2118,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B50E24F-02BF-4852-9ABA-EC20BBB2E158}">
-  <dimension ref="B2:L33"/>
-  <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.75" customWidth="1"/>
-    <col min="2" max="2" width="11.625" customWidth="1"/>
-    <col min="3" max="3" width="16.125" customWidth="1"/>
-    <col min="4" max="4" width="17.375" customWidth="1"/>
-    <col min="5" max="5" width="14.375" customWidth="1"/>
-    <col min="6" max="6" width="12.125" customWidth="1"/>
-    <col min="7" max="8" width="15.375" customWidth="1"/>
-    <col min="9" max="9" width="5.75" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="J2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3" s="20">
-        <f>1502.33/1000</f>
-        <v>1.5023299999999999</v>
-      </c>
-      <c r="L3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B4" s="7">
-        <v>0</v>
-      </c>
-      <c r="C4" s="12">
-        <v>4.51531200000003</v>
-      </c>
-      <c r="D4" s="5">
-        <f>F4*(C4/E4)</f>
-        <v>0</v>
-      </c>
-      <c r="E4" s="5">
-        <v>4.5600000000000307</v>
-      </c>
-      <c r="F4" s="5">
-        <v>0</v>
-      </c>
-      <c r="G4" s="7">
-        <v>0</v>
-      </c>
-      <c r="H4" s="5">
-        <v>10.14973</v>
-      </c>
-      <c r="J4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <f>1395.43/1000</f>
-        <v>1.3954300000000002</v>
-      </c>
-      <c r="L4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" s="6">
-        <v>0.91666666666424135</v>
-      </c>
-      <c r="C5" s="12">
-        <v>6.3592699999999365</v>
-      </c>
-      <c r="D5" s="5">
-        <f t="shared" ref="D5:D14" si="0">F5*(C5/E5)</f>
-        <v>9.8899999999769502E-3</v>
-      </c>
-      <c r="E5" s="8">
-        <v>6.4299999999999358</v>
-      </c>
-      <c r="F5" s="18">
-        <v>9.9999999999766942E-3</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0.91666666666424135</v>
-      </c>
-      <c r="H5" s="5">
-        <v>7.7853500000000002</v>
-      </c>
-      <c r="J5" t="s">
-        <v>3</v>
-      </c>
-      <c r="K5" s="11">
-        <v>35</v>
-      </c>
-      <c r="L5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B6" s="6">
-        <v>1.8611111111094942</v>
-      </c>
-      <c r="C6" s="12">
-        <v>7.444318000000095</v>
-      </c>
-      <c r="D6" s="5">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="E6" s="8">
-        <v>7.5800000000000978</v>
-      </c>
-      <c r="F6" s="17">
-        <v>0</v>
-      </c>
-      <c r="G6" s="6">
-        <v>1.8611111111094942</v>
-      </c>
-      <c r="H6" s="5">
-        <v>6.0335299999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" s="6">
-        <v>5.8819444444452529</v>
-      </c>
-      <c r="C7" s="12">
-        <v>10.774652000000156</v>
-      </c>
-      <c r="D7" s="5">
-        <f t="shared" si="0"/>
-        <v>1.9484000000300698E-2</v>
-      </c>
-      <c r="E7" s="8">
-        <v>11.060000000000159</v>
-      </c>
-      <c r="F7" s="17">
-        <v>2.000000000030866E-2</v>
-      </c>
-      <c r="G7" s="6">
-        <v>5.8819444444452529</v>
-      </c>
-      <c r="H7" s="5">
-        <v>3.96672</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" s="6">
-        <v>7.8888888888905058</v>
-      </c>
-      <c r="C8" s="12">
-        <v>12.066321999999785</v>
-      </c>
-      <c r="D8" s="5">
-        <f t="shared" si="0"/>
-        <v>2.9453999999931358E-2</v>
-      </c>
-      <c r="E8" s="8">
-        <v>12.289999999999779</v>
-      </c>
-      <c r="F8" s="17">
-        <v>2.9999999999930083E-2</v>
-      </c>
-      <c r="G8" s="6">
-        <v>7.8888888888905058</v>
-      </c>
-      <c r="H8" s="5">
-        <v>3.6516799999999998</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" s="6">
-        <v>9.875</v>
-      </c>
-      <c r="C9" s="12">
-        <v>12.870088000000043</v>
-      </c>
-      <c r="D9" s="5">
-        <f t="shared" si="0"/>
-        <v>9.8319999999770848E-3</v>
-      </c>
-      <c r="E9" s="8">
-        <v>13.090000000000046</v>
-      </c>
-      <c r="F9" s="17">
-        <v>9.9999999999766942E-3</v>
-      </c>
-      <c r="G9" s="6">
-        <v>9.875</v>
-      </c>
-      <c r="H9" s="5">
-        <v>3.5996700000000001</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" s="6">
-        <v>13.875</v>
-      </c>
-      <c r="C10" s="12">
-        <v>13.143288000000254</v>
-      </c>
-      <c r="D10" s="5">
-        <f t="shared" si="0"/>
-        <v>3.3210767469427079E-13</v>
-      </c>
-      <c r="E10" s="8">
-        <v>14.060000000000272</v>
-      </c>
-      <c r="F10" s="17">
-        <v>3.5527136788005009E-13</v>
-      </c>
-      <c r="G10" s="6">
-        <v>13.875</v>
-      </c>
-      <c r="H10" s="5">
-        <v>3.56338</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
-        <v>16.861111111109494</v>
-      </c>
-      <c r="C11" s="12">
-        <v>12.947249999999734</v>
-      </c>
-      <c r="D11" s="5">
-        <f t="shared" si="0"/>
-        <v>9.1499999999786769E-3</v>
-      </c>
-      <c r="E11" s="8">
-        <v>14.149999999999707</v>
-      </c>
-      <c r="F11" s="17">
-        <v>9.9999999999766942E-3</v>
-      </c>
-      <c r="G11" s="6">
-        <v>16.861111111109494</v>
-      </c>
-      <c r="H11" s="5">
-        <v>3.54481</v>
-      </c>
-      <c r="K11" s="16"/>
-    </row>
-    <row r="12" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B12" s="6">
-        <v>19.861111111109494</v>
-      </c>
-      <c r="C12" s="12">
-        <v>12.757108000000079</v>
-      </c>
-      <c r="D12" s="5">
-        <f t="shared" si="0"/>
-        <v>3.6087999999595374E-2</v>
-      </c>
-      <c r="E12" s="8">
-        <v>14.140000000000086</v>
-      </c>
-      <c r="F12" s="17">
-        <v>3.9999999999551505E-2</v>
-      </c>
-      <c r="G12" s="6">
-        <v>19.861111111109494</v>
-      </c>
-      <c r="H12" s="5">
-        <v>3.55558</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="6">
-        <v>23.861111111109494</v>
-      </c>
-      <c r="C13" s="12">
-        <v>12.940480000000202</v>
-      </c>
-      <c r="D13" s="5">
-        <f t="shared" si="0"/>
-        <v>3.4879999999918712E-2</v>
-      </c>
-      <c r="E13" s="8">
-        <v>14.840000000000231</v>
-      </c>
-      <c r="F13" s="17">
-        <v>3.9999999999906777E-2</v>
-      </c>
-      <c r="G13" s="6">
-        <v>23.861111111109494</v>
-      </c>
-      <c r="H13" s="5">
-        <v>3.5422699999999998</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B14" s="6">
-        <v>27.875</v>
-      </c>
-      <c r="C14" s="13">
-        <v>14.122536999999936</v>
-      </c>
-      <c r="D14" s="5">
-        <f t="shared" si="0"/>
-        <v>8.7229999999796706E-3</v>
-      </c>
-      <c r="E14">
-        <v>16.189999999999927</v>
-      </c>
-      <c r="F14" s="19">
-        <v>9.9999999999766942E-3</v>
-      </c>
-      <c r="G14" s="6">
-        <v>27.875</v>
-      </c>
-      <c r="H14">
-        <v>3.5102899999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="4:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="E22" s="10"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="4:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="D23" s="14"/>
-      <c r="E23" s="9"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-    </row>
-    <row r="24" spans="4:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="D24" s="14"/>
-      <c r="E24" s="9"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-    </row>
-    <row r="25" spans="4:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="D25" s="14"/>
-      <c r="E25" s="9"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-    </row>
-    <row r="26" spans="4:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="D26" s="14"/>
-      <c r="E26" s="9"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-    </row>
-    <row r="27" spans="4:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="D27" s="14"/>
-      <c r="E27" s="9"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-    </row>
-    <row r="28" spans="4:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="D28" s="14"/>
-      <c r="E28" s="9"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-    </row>
-    <row r="29" spans="4:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="D29" s="15"/>
-      <c r="E29" s="9"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-    </row>
-    <row r="30" spans="4:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="D30" s="15"/>
-      <c r="E30" s="9"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-    </row>
-    <row r="31" spans="4:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="D31" s="15"/>
-      <c r="E31" s="9"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-    </row>
-    <row r="32" spans="4:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="D32" s="15"/>
-      <c r="E32" s="9"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-    </row>
-    <row r="33" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{963B64C9-FCCA-4712-AAF9-7029EBE0A6AA}">
-  <dimension ref="B2:L33"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="2.75" customWidth="1"/>
-    <col min="2" max="2" width="11.625" customWidth="1"/>
-    <col min="3" max="3" width="16.125" customWidth="1"/>
-    <col min="4" max="4" width="17.375" customWidth="1"/>
-    <col min="5" max="5" width="14.375" customWidth="1"/>
-    <col min="6" max="6" width="12.125" customWidth="1"/>
-    <col min="7" max="8" width="15.375" customWidth="1"/>
-    <col min="9" max="9" width="5.75" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="29.625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="H2" s="2"/>
-      <c r="J2" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="K2" s="1"/>
-      <c r="L2" s="1"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-      <c r="G3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H3" t="s">
-        <v>9</v>
-      </c>
-      <c r="J3" t="s">
-        <v>0</v>
-      </c>
-      <c r="K3">
-        <f>1498.07/1000</f>
-        <v>1.49807</v>
-      </c>
-      <c r="L3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B4" s="7">
-        <v>0</v>
-      </c>
-      <c r="C4" s="12">
-        <v>4.5021399999999838</v>
-      </c>
-      <c r="D4" s="5">
-        <f>F4*(C4/E4)</f>
-        <v>3.9319999999908359E-2</v>
-      </c>
-      <c r="E4" s="5">
-        <v>4.5799999999999841</v>
-      </c>
-      <c r="F4" s="5">
-        <v>3.9999999999906777E-2</v>
-      </c>
-      <c r="G4" s="7">
-        <v>0</v>
-      </c>
-      <c r="H4" s="5">
-        <v>10.086679999999999</v>
-      </c>
-      <c r="J4" t="s">
-        <v>1</v>
-      </c>
-      <c r="K4">
-        <v>1.3964099999999999</v>
-      </c>
-      <c r="L4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B5" s="6">
-        <v>0.91666666667151731</v>
-      </c>
-      <c r="C5" s="12">
-        <v>6.4484799999999884</v>
-      </c>
-      <c r="D5" s="5">
-        <f t="shared" ref="D5:D14" si="0">F5*(C5/E5)</f>
-        <v>1.9659999999604948E-2</v>
-      </c>
-      <c r="E5" s="8">
-        <v>6.5599999999999881</v>
-      </c>
-      <c r="F5" s="18">
-        <v>1.9999999999598117E-2</v>
-      </c>
-      <c r="G5" s="6">
-        <v>0.91666666666424135</v>
-      </c>
-      <c r="H5" s="5">
-        <v>7.7757100000000001</v>
-      </c>
-      <c r="J5" t="s">
-        <v>3</v>
-      </c>
-      <c r="K5" s="11">
-        <v>35</v>
-      </c>
-      <c r="L5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B6" s="6">
-        <v>1.8611111111167702</v>
-      </c>
-      <c r="C6" s="12">
-        <v>7.6620359999998957</v>
-      </c>
-      <c r="D6" s="5">
-        <f t="shared" si="0"/>
-        <v>1.9596000000302424E-2</v>
-      </c>
-      <c r="E6" s="8">
-        <v>7.8199999999998937</v>
-      </c>
-      <c r="F6" s="17">
-        <v>2.000000000030866E-2</v>
-      </c>
-      <c r="G6" s="6">
-        <v>1.8611111111094942</v>
-      </c>
-      <c r="H6" s="5">
-        <v>6.0335299999999998</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B7" s="6">
-        <v>5.8819444444452529</v>
-      </c>
-      <c r="C7" s="12">
-        <v>11.022479999999867</v>
-      </c>
-      <c r="D7" s="5">
-        <f t="shared" si="0"/>
-        <v>1.9439999999954695E-2</v>
-      </c>
-      <c r="E7" s="8">
-        <v>11.339999999999861</v>
-      </c>
-      <c r="F7" s="17">
-        <v>1.9999999999953388E-2</v>
-      </c>
-      <c r="G7" s="6">
-        <v>5.8819444444452529</v>
-      </c>
-      <c r="H7" s="5">
-        <v>3.84185</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B8" s="6">
-        <v>7.8611111111167702</v>
-      </c>
-      <c r="C8" s="12">
-        <v>12.376760000000006</v>
-      </c>
-      <c r="D8" s="5">
-        <f t="shared" si="0"/>
-        <v>9.784000000324795E-3</v>
-      </c>
-      <c r="E8" s="8">
-        <v>12.650000000000006</v>
-      </c>
-      <c r="F8" s="17">
-        <v>1.0000000000331966E-2</v>
-      </c>
-      <c r="G8" s="6">
-        <v>7.8888888888905058</v>
-      </c>
-      <c r="H8" s="5">
-        <v>3.6354899999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B9" s="6">
-        <v>9.875</v>
-      </c>
-      <c r="C9" s="12">
-        <v>13.180049999999806</v>
-      </c>
-      <c r="D9" s="5">
-        <f t="shared" si="0"/>
-        <v>7.8103999999817972E-2</v>
-      </c>
-      <c r="E9" s="8">
-        <v>13.499999999999801</v>
-      </c>
-      <c r="F9" s="17">
-        <v>7.9999999999813554E-2</v>
-      </c>
-      <c r="G9" s="6">
-        <v>9.875</v>
-      </c>
-      <c r="H9" s="5">
-        <v>3.57003</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B10" s="6">
-        <v>13.875</v>
-      </c>
-      <c r="C10" s="12">
-        <v>14.306147999999959</v>
-      </c>
-      <c r="D10" s="5">
-        <f t="shared" si="0"/>
-        <v>4.7340000000226042E-2</v>
-      </c>
-      <c r="E10" s="8">
-        <v>15.109999999999957</v>
-      </c>
-      <c r="F10" s="17">
-        <v>5.0000000000238742E-2</v>
-      </c>
-      <c r="G10" s="6">
-        <v>13.875</v>
-      </c>
-      <c r="H10" s="5">
-        <v>3.5518999999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B11" s="6">
-        <v>16.857638888890506</v>
-      </c>
-      <c r="C11" s="12">
-        <v>14.313178999999911</v>
-      </c>
-      <c r="D11" s="5">
-        <f t="shared" si="0"/>
-        <v>4.5904999999893011E-2</v>
-      </c>
-      <c r="E11" s="8">
-        <v>15.589999999999904</v>
-      </c>
-      <c r="F11" s="17">
-        <v>4.9999999999883471E-2</v>
-      </c>
-      <c r="G11" s="6">
-        <v>16.861111111109494</v>
-      </c>
-      <c r="H11" s="5">
-        <v>3.52163</v>
-      </c>
-      <c r="K11" s="16"/>
-    </row>
-    <row r="12" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B12" s="6">
-        <v>19.857638888890506</v>
-      </c>
-      <c r="C12" s="12">
-        <v>13.984840000000107</v>
-      </c>
-      <c r="D12" s="5">
-        <f t="shared" si="0"/>
-        <v>2.6807999999620049E-2</v>
-      </c>
-      <c r="E12" s="8">
-        <v>15.650000000000119</v>
-      </c>
-      <c r="F12" s="17">
-        <v>2.9999999999574811E-2</v>
-      </c>
-      <c r="G12" s="6">
-        <v>19.861111111109494</v>
-      </c>
-      <c r="H12" s="5">
-        <v>3.5405700000000002</v>
-      </c>
-    </row>
-    <row r="13" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="6">
-        <v>23.857638888890506</v>
-      </c>
-      <c r="C13" s="12">
-        <v>13.766903999999833</v>
-      </c>
-      <c r="D13" s="5">
-        <f t="shared" si="0"/>
-        <v>0.41397599999966106</v>
-      </c>
-      <c r="E13" s="8">
-        <v>15.629999999999811</v>
-      </c>
-      <c r="F13" s="17">
-        <v>0.46999999999961517</v>
-      </c>
-      <c r="G13" s="6">
-        <v>23.861111111109494</v>
-      </c>
-      <c r="H13" s="5">
-        <v>3.55118</v>
-      </c>
-    </row>
-    <row r="14" spans="2:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B14" s="6">
-        <v>27.864583333335759</v>
-      </c>
-      <c r="C14" s="13">
-        <v>15.117164000000109</v>
-      </c>
-      <c r="D14" s="5">
-        <f t="shared" si="0"/>
-        <v>1.7763999999958598E-2</v>
-      </c>
-      <c r="E14">
-        <v>17.020000000000124</v>
-      </c>
-      <c r="F14" s="19">
-        <v>1.9999999999953388E-2</v>
-      </c>
-      <c r="G14" s="6">
-        <v>27.875</v>
-      </c>
-      <c r="H14">
-        <v>3.50779</v>
-      </c>
-    </row>
-    <row r="22" spans="4:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="E22" s="10"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="4"/>
-    </row>
-    <row r="23" spans="4:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="D23" s="14"/>
-      <c r="E23" s="9"/>
-      <c r="G23" s="15"/>
-      <c r="H23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
-    </row>
-    <row r="24" spans="4:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="D24" s="14"/>
-      <c r="E24" s="9"/>
-      <c r="G24" s="15"/>
-      <c r="H24" s="9"/>
-      <c r="K24" s="9"/>
-      <c r="L24" s="9"/>
-    </row>
-    <row r="25" spans="4:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="D25" s="14"/>
-      <c r="E25" s="9"/>
-      <c r="G25" s="15"/>
-      <c r="H25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
-    </row>
-    <row r="26" spans="4:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="D26" s="14"/>
-      <c r="E26" s="9"/>
-      <c r="G26" s="15"/>
-      <c r="H26" s="9"/>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
-    </row>
-    <row r="27" spans="4:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="D27" s="14"/>
-      <c r="E27" s="9"/>
-      <c r="G27" s="15"/>
-      <c r="H27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-    </row>
-    <row r="28" spans="4:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="D28" s="14"/>
-      <c r="E28" s="9"/>
-      <c r="G28" s="15"/>
-      <c r="H28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-    </row>
-    <row r="29" spans="4:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="D29" s="15"/>
-      <c r="E29" s="9"/>
-      <c r="G29" s="15"/>
-      <c r="H29" s="9"/>
-      <c r="K29" s="9"/>
-      <c r="L29" s="9"/>
-    </row>
-    <row r="30" spans="4:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="D30" s="15"/>
-      <c r="E30" s="9"/>
-      <c r="G30" s="15"/>
-      <c r="H30" s="9"/>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
-    </row>
-    <row r="31" spans="4:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="D31" s="15"/>
-      <c r="E31" s="9"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="9"/>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
-    </row>
-    <row r="32" spans="4:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="D32" s="15"/>
-      <c r="E32" s="9"/>
-      <c r="G32" s="15"/>
-      <c r="H32" s="9"/>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-    </row>
-    <row r="33" spans="4:12" x14ac:dyDescent="0.25">
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="9"/>
-      <c r="K33" s="9"/>
-      <c r="L33" s="9"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AA6ED3AE-2AE6-40B8-A619-1A329F8EF087}">
   <dimension ref="B2:L25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H4" sqref="H4:H14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K21" sqref="K21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -3437,7 +2471,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3C160521-EBF9-458D-BDC1-CF0121090C29}">
   <dimension ref="B2:L22"/>
   <sheetViews>
@@ -3791,7 +2825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAFC84B1-352E-4FA0-A262-B32F8F2B1408}">
   <dimension ref="B2:L14"/>
   <sheetViews>

</xml_diff>